<commit_message>
skriver til nytt excel ark
</commit_message>
<xml_diff>
--- a/resultat.xlsx
+++ b/resultat.xlsx
@@ -1,56 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\OneDrive\Dokumenter\DIKU\DIKU\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31D597AC-A18B-4527-B453-19CF527EEB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{812F2556-BB88-4699-9A89-BA220739851F}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -383,13 +419,561 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D4B94F-7B54-4A4E-A78F-ABFE0AADD56F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <cols>
+    <col width="16.44140625" customWidth="1" min="1" max="1"/>
+    <col width="13.5546875" customWidth="1" min="5" max="5"/>
+    <col width="15.33203125" bestFit="1" customWidth="1" min="7" max="8"/>
+    <col width="14.6640625" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="14.33203125" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="14.88671875" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="16.88671875" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="14.88671875" bestFit="1" customWidth="1" min="13" max="13"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Søkeord:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Treff- LUK</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Treff-LUF</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Treff-LUG</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Treff-søkeord</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Totale treff</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Mulige treff-LUK</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Mulige treff-LUF</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Mulige treff-LUG</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Mulig treff-søkeord</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Mulig totale treff</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>digital tvilling</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>48</v>
+      </c>
+      <c r="J2" t="n">
+        <v>48</v>
+      </c>
+      <c r="K2" t="n">
+        <v>48</v>
+      </c>
+      <c r="L2" t="n">
+        <v>144</v>
+      </c>
+      <c r="M2" t="n">
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>virtuell</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> vr </t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ar </t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> xr </t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>hololens</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>big room</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>revit</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>programmvare</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>trimble</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> bim </t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>digital samhand</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>digitalisering</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>modell</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>7</v>
+      </c>
+      <c r="C15" t="n">
+        <v>7</v>
+      </c>
+      <c r="D15" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>kunstlig intelligens</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ice </t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> vdc </t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>concurrent</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>engineering</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ipd </t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>lean</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>maskinlæring</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ai </t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ifc </t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nye sheets med resultater
</commit_message>
<xml_diff>
--- a/resultat.xlsx
+++ b/resultat.xlsx
@@ -6,7 +6,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Statistikk" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name=" BIM" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="modell" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -210,7 +212,7 @@
           </dPt>
           <cat>
             <strRef>
-              <f>'Ark1'!$G$1:$H$1</f>
+              <f>Statistikk!$G$1:$H$1</f>
               <strCache>
                 <ptCount val="2"/>
                 <pt idx="0">
@@ -224,7 +226,7 @@
           </cat>
           <val>
             <numRef>
-              <f>'Ark1'!$G$2:$H$2</f>
+              <f>Statistikk!$G$2:$H$2</f>
               <numCache>
                 <formatCode>General</formatCode>
                 <ptCount val="2"/>
@@ -336,7 +338,7 @@
           <invertIfNegative val="0"/>
           <cat>
             <strRef>
-              <f>'Ark1'!$G$1:$H$1</f>
+              <f>Statistikk!$G$1:$H$1</f>
               <strCache>
                 <ptCount val="2"/>
                 <pt idx="0">
@@ -350,7 +352,7 @@
           </cat>
           <val>
             <numRef>
-              <f>'Ark1'!$G$2:$H$2</f>
+              <f>Statistikk!$G$2:$H$2</f>
               <numCache>
                 <formatCode>General</formatCode>
                 <ptCount val="2"/>
@@ -858,7 +860,7 @@
   <dimension ref="A1:Y24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -1398,4 +1400,228 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BYTS1401</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BYFE1201</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BYFE3100</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BYTS1401</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BYFE1201</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EMPE2500</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BYPE1500</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BYFE1000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BYFE1201</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BYPE2200</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BYTS1401</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BYPE2700</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BYPE2700</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DAVE3705</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>BYFE1201</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BYTS2691</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>EMFE1000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>EMTS2200</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BYVE3200</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>EMPE2500</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>EMTS2300</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>FEPE2100</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EMVE3700</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>EMVE3700</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>EMVE3700</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DAVE3705</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
hadde skrivefeil i nøkkelord, rettet opp
</commit_message>
<xml_diff>
--- a/resultat.xlsx
+++ b/resultat.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Statistikk" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name=" BIM" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="digital" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="modell" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="samarbeid" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="teknologi" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="programm" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="programvare" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name=" BIM" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="digital" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="modell" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="samarbeid" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="teknologi" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="programm" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -963,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H2">
         <f>M2-G2</f>
@@ -1121,20 +1122,20 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>programmvare</t>
+          <t>programvare</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -1543,6 +1544,221 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LUF:</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LUG:</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Emnekode:</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Emnenavn:</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Læringsutbytte</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Emnekode:</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Emnenavn:</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Læringsutbytte</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>Emnekode:</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>Emnenavn:</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Læringsutbytte</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n"/>
+      <c r="C3" s="1" t="n"/>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>BYVE3401</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Areal- og transportplanlegging</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan utarbeide en reguleringsplan med tilhørende reguleringsbestemmelser og planbeskrivelse i samsvar med Miljøverndepartementets veiledning for reguleringsplaner samt overordnede føringer prinsippene for utforming av reguleringsplaner ved bruk av egnet programvare NovaPoint Areal Focus Arealplanlegging eller tilsvarende med tilhørende tekniske planer for Veg VA plantegning lengdeprofiler og tverrprofiler utføre konsekvensanalyser for områdereguleringsplan og ROS-analyse for detaljreguleringsplan utføre grunnleggende trafikktekniske beregninger og analyser</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>EMPE1500</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Fysikk</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan identifisere krefter og beregne kraftmomenter anvende Newtons 2 lov og spinnsatsen på konkrete fysiske problemer beskrive bevegelse matematisk blant annet ved hjelp av egnet programvare løse likevektproblemer for stive legemer</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>EMPE2500</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Bygningssimulering</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan utføre grunnleggende beregninger av varmetransport U-verdier kuldebro infiltrasjon og av effekt- og energibehovs med enkle formelverk håndtere bygningsinformasjonsmodeller BIM deriblant overføre data til programvare for simulering og miljøvurdering utføre dynamisk modellering av bygnings- og klimatekniske systemer for optimalt inneklima effekt- og energibehov ved bruk av simuleringsprogrammer som SIMIEN TEK-sjekk eller tilsvarende utføre energimerking av bygg vurdere inneklima termisk komfort og dagslysforhold utfra beregningene</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
+      <c r="I5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>EMTS2600</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>Inneklima og måleteknikk</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan vurdere usikkerhet i alle typer målinger av inneklimaparametere og sette opp et usikkerhetsbudsjett håndtere spørreundersøkelser om inneklima ved hjelp av «Ørebroskjemaet» og tolke resultatet beregne nødvendige luftmengder ut ifra massebalanser og reaksjonskinetikk utføre målinger av inneklimaparametere som luftskifte luftkvalitet termiske akustiske og aktiniske forhold inkludert radon og sammenlikne dem med myndighetskrav vurdere materialbruken med hensyn på inneklimakvalitet og miljøbelastning foreta en mikrobiologisk analyse av en bygning spesielt med hensyn på muggsopp bruke Mollierediagram for å beregne duggpunkt og andre termodynamiske data for fuktig luft anvende programvare for inneklimasimuleringer designe for optimalt vedlikehold for å unngå Legionellavekst i varmtvannssystemer og kjøletårn designe våtrom</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="n"/>
+      <c r="H6" s="1" t="n"/>
+      <c r="I6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>EMVE3500</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>Varme, ventilasjon og sanitærteknikk</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan velge energikilderenergiforsyning som tilfredsstiller myndighetskrav gjennomføre energi- og inneklimaberegninger med relevant programvare utarbeide kravspesifikasjon for oppvarmingssystemer prosjekteredimensjonere energieffektive vannbårne oppvarmingsanlegg prosjekteredimensjonere energieffektive kjølesystemer utarbeide kravspesifikasjon for ventilasjonssystemer prosjekteredimensjonere energieffektive ventilasjonsanlegg herunder aggregat og kanalnett prosjekteredimensjonere ventilasjonsløsninger på rom nivå som gir akseptabelt inneklima med hensyn på temperatur trekk luftkvalitet og lyd prosjekteredimensjonere sanitærtekniske installasjoner innomhus vannforsyning og avløp prosjekteredimensjonere varmtvannsforsyningsanlegg</t>
+        </is>
+      </c>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1735,7 +1951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1905,7 +2121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2298,7 +2514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2460,281 +2676,6 @@
       <c r="I4" s="1" t="inlineStr">
         <is>
           <t>Studenten har kompetanse til å ta riktige avgjørelser for å få ønsket resultat innenfor de definerte kostnads- og kvalitetsrammer har kompetanse til å kunne gjennomføre evalueringer og velge riktige og tilpassede modeller for prosjektorganisering basert på prosjektets varighet størrelse og kompleksitet kan samarbeide og bidra til tverrfaglig teamsamarbeid kunne relatere forutsetninger for å lykkes i prosjektarbeid med ens arbeidssituasjon</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="50" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="50" customWidth="1" min="9" max="9"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>LUK:</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>LUF:</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>LUG:</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Emnekode:</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>Emnenavn:</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>Læringsutbytte</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Emnekode:</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>Emnenavn:</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>Læringsutbytte</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>Emnekode:</t>
-        </is>
-      </c>
-      <c r="H2" s="1" t="inlineStr">
-        <is>
-          <t>Emnenavn:</t>
-        </is>
-      </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>Læringsutbytte</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>BYPE2700</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="inlineStr">
-        <is>
-          <t>Prosjektstryring</t>
-        </is>
-      </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>Studenten har kunnskap om hvordan man identifiserer og analyserer utfordringer knyttet til prosjektets initieringsfase og kan definere forutsetninger for prosjektsuksess har grunnleggende kunnskap om avhengigheten mellom prosjekteiers forretningsmessige mål bygningsdesign teknologibruk og støttefunksjoner og hvordan dette forstås i et helhetlig perspektiv forstår prosjekteringsprosessen og dens plass i den samlede byggeprosessen har kunnskap om produkt som brukes i prosjekteringsprosess og hva som utgjør verdi i dem har kunnskap om kompleksitet i byggeprosjekter behovet for tverrfaglig samarbeid og håndtering av grensesnitt forstår viktigheten av profesjonell styring av prosjekteringsprosess for å gjøre prosjektet egnet for bruker og eiers formål har inngående kunnskap om de vanligste tids- og kostnadsestimeringsmetodene har inngående kunnskap om analysemetoder som livssyklus- kostnads- og interessentanalyse kan beskrive hovedkategoriene av prosjektorganisasjonsstrukturer prosjekt klassisk og matrise og forstår fordeler og ulemper ved de forskjellige modellene har kunnskap om forskjellige kontrakts- og prosjektleveringsmodeller inkludert nye innovative samarbeidsmodeller</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>BYFE1201</t>
-        </is>
-      </c>
-      <c r="E3" s="1" t="inlineStr">
-        <is>
-          <t>Byggfaglig innføring</t>
-        </is>
-      </c>
-      <c r="F3" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan samarbeide i gruppeprosjekt foreta faktainnsamling analysere designe implementere og anvende de teknologier som trengs for å løse konkrete tverrfaglige oppgaver integrere kunnskapen om de forskjellige praktiske tekniske og miljømessige krav som stilles til bygg slik at det resulterer i en helhetlig fungerende løsning planlegge og prosjektere enkle konstruksjoner i trehus utføre enkle varme- og fukttransportberegninger for bygningsdeler fremstille enkle byggetekniske tegninger ved hjelp av BIM-verktøy presentere resultater ved hjelp av tegninger skriftlige rapporter og muntlige presentasjoner</t>
-        </is>
-      </c>
-      <c r="G3" s="1" t="inlineStr">
-        <is>
-          <t>BYTS3900</t>
-        </is>
-      </c>
-      <c r="H3" s="1" t="inlineStr">
-        <is>
-          <t>Bacheloroppgave</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>Studenten behersker å arbeide i team med planlegging og gjennomføring av prosjekt viser selvstendighet og initiativ kreativitet og innovasjon vurderer teknologiske løsninger i en livsløps- miljømessig samfunnsmessig og økonomisk sammenheng har informasjonskompetanse vet hvorfor man skal søke etter kvalitetssikrede kunnskapskilder og hvorfor korrekt henvisning til kilder er viktig analyserer og kvalitetssikrer resultatene og viser evne til refleksjon</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>DAVE3710</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="inlineStr">
-        <is>
-          <t>Akademisk Engelsk</t>
-        </is>
-      </c>
-      <c r="C4" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan på engelsk beskrive teknologens arbeid innenfor et valgt teknologiområde beskrive forskning og utvikling innenfor et valgt teknologiområdeforklare retoriske virkemidler og argumentasjon</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>BYTS1401</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>Byggeteknikk</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan utføre manuelle tegninger av enkle legemer i vanlige projeksjoner kan fremstille ulike byggetekniske tegninger både manuelt og ved hjelp av 3D-modelleringsprogrammer kan gjøre valg av materialer løsninger og komponenter for småhusbebyggelse i tre og gi begrunnelse for hvorfor disse løsningene er valgt kan utarbeide en postbeskrivelse etter NS3420 og beregne byggekostnader ved hjelp av BIM-teknologi</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>EMTS2200</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>Strømningsteknikk</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan bidra i arbeidet med å utvikle ny teknologi med bakgrunn i en forståelse for matematisk modellering og løsning av fysiske problemer løse koblede problemer knyttet til både strømningsteknikk varme- og massetransport og termodynamikk vurdere nøyaktigheten i beregningene og gyldigheten til den matematiske modellen</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n"/>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="inlineStr">
-        <is>
-          <t>DAVE3710</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>Akademisk Engelsk</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan på engelsk bruke korrekt terminologi innenfor teknologirelaterte emner generelt og innenfor et valgt fagområde spesielt presentere teknologi og relaterte prosesser utforme og skrive tekniske og akademiske tekster på engelsk i tråd med internasjonale konvensjoner og uttrykksmåte finne relevante kunnskapskilder vurdere kvaliteten på kilder og refererer til kilder i henhold til etablerte standarder bruke muntlig engelsk i faglige diskusjoner</t>
-        </is>
-      </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>EMTS2300</t>
-        </is>
-      </c>
-      <c r="H5" s="1" t="inlineStr">
-        <is>
-          <t>Varmetransport</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan bidra i arbeidet med å utvikle ny teknologi med bakgrunn i en forståelse for matematisk modellering og løsning av fysiske problemer løse koblede problemer knyttet til både varmetransport termodynamikk og fluidmekanikk strømningslære Dette vil være et grunnlag for beregning av for eksempel et byggs effekt- og energibehov vurdere om beregningsresultater er rimelige</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="1" t="n"/>
-      <c r="E6" s="1" t="n"/>
-      <c r="F6" s="1" t="n"/>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>EMVE3700</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
-        <is>
-          <t>Numerisk varme- og strømningsteknikk</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>Studenten kan bidra i arbeidet med å utvikle ny teknologi med bakgrunn i en forståelse for matematisk modellering og løsning av fysiske problemer kan løse koblede problemer knyttet til både varmetransport termodynamikk og fluidmekanikk strømningslære Dette vil være et grunnlag for beregning av for eksempel et byggs effekt- og energibehov kan vurdere om beregningsresultater er rimelige sikre ferdigheter i en for fremtidens ingeniører aktuell arbeidsmåte</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
-      <c r="E7" s="1" t="n"/>
-      <c r="F7" s="1" t="n"/>
-      <c r="G7" s="1" t="inlineStr">
-        <is>
-          <t>EMTS3900</t>
-        </is>
-      </c>
-      <c r="H7" s="1" t="inlineStr">
-        <is>
-          <t>Bacheloroppgave</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>Studenten behersker å arbeide i team med planlegging og gjennomføring av prosjekt viser selvstendighet og initiativ kreativitet og innovasjon vurderer teknologiske løsninger i en livsløps- miljømessig samfunnsmessig og økonomisk sammenheng analyserer og kvalitetssikrer resultatene og viser evne til refleksjon</t>
         </is>
       </c>
     </row>
@@ -2841,6 +2782,281 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
+          <t>BYPE2700</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Prosjektstryring</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>Studenten har kunnskap om hvordan man identifiserer og analyserer utfordringer knyttet til prosjektets initieringsfase og kan definere forutsetninger for prosjektsuksess har grunnleggende kunnskap om avhengigheten mellom prosjekteiers forretningsmessige mål bygningsdesign teknologibruk og støttefunksjoner og hvordan dette forstås i et helhetlig perspektiv forstår prosjekteringsprosessen og dens plass i den samlede byggeprosessen har kunnskap om produkt som brukes i prosjekteringsprosess og hva som utgjør verdi i dem har kunnskap om kompleksitet i byggeprosjekter behovet for tverrfaglig samarbeid og håndtering av grensesnitt forstår viktigheten av profesjonell styring av prosjekteringsprosess for å gjøre prosjektet egnet for bruker og eiers formål har inngående kunnskap om de vanligste tids- og kostnadsestimeringsmetodene har inngående kunnskap om analysemetoder som livssyklus- kostnads- og interessentanalyse kan beskrive hovedkategoriene av prosjektorganisasjonsstrukturer prosjekt klassisk og matrise og forstår fordeler og ulemper ved de forskjellige modellene har kunnskap om forskjellige kontrakts- og prosjektleveringsmodeller inkludert nye innovative samarbeidsmodeller</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>BYFE1201</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Byggfaglig innføring</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan samarbeide i gruppeprosjekt foreta faktainnsamling analysere designe implementere og anvende de teknologier som trengs for å løse konkrete tverrfaglige oppgaver integrere kunnskapen om de forskjellige praktiske tekniske og miljømessige krav som stilles til bygg slik at det resulterer i en helhetlig fungerende løsning planlegge og prosjektere enkle konstruksjoner i trehus utføre enkle varme- og fukttransportberegninger for bygningsdeler fremstille enkle byggetekniske tegninger ved hjelp av BIM-verktøy presentere resultater ved hjelp av tegninger skriftlige rapporter og muntlige presentasjoner</t>
+        </is>
+      </c>
+      <c r="G3" s="1" t="inlineStr">
+        <is>
+          <t>BYTS3900</t>
+        </is>
+      </c>
+      <c r="H3" s="1" t="inlineStr">
+        <is>
+          <t>Bacheloroppgave</t>
+        </is>
+      </c>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>Studenten behersker å arbeide i team med planlegging og gjennomføring av prosjekt viser selvstendighet og initiativ kreativitet og innovasjon vurderer teknologiske løsninger i en livsløps- miljømessig samfunnsmessig og økonomisk sammenheng har informasjonskompetanse vet hvorfor man skal søke etter kvalitetssikrede kunnskapskilder og hvorfor korrekt henvisning til kilder er viktig analyserer og kvalitetssikrer resultatene og viser evne til refleksjon</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>DAVE3710</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Akademisk Engelsk</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan på engelsk beskrive teknologens arbeid innenfor et valgt teknologiområde beskrive forskning og utvikling innenfor et valgt teknologiområdeforklare retoriske virkemidler og argumentasjon</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>BYTS1401</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Byggeteknikk</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan utføre manuelle tegninger av enkle legemer i vanlige projeksjoner kan fremstille ulike byggetekniske tegninger både manuelt og ved hjelp av 3D-modelleringsprogrammer kan gjøre valg av materialer løsninger og komponenter for småhusbebyggelse i tre og gi begrunnelse for hvorfor disse løsningene er valgt kan utarbeide en postbeskrivelse etter NS3420 og beregne byggekostnader ved hjelp av BIM-teknologi</t>
+        </is>
+      </c>
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>EMTS2200</t>
+        </is>
+      </c>
+      <c r="H4" s="1" t="inlineStr">
+        <is>
+          <t>Strømningsteknikk</t>
+        </is>
+      </c>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan bidra i arbeidet med å utvikle ny teknologi med bakgrunn i en forståelse for matematisk modellering og løsning av fysiske problemer løse koblede problemer knyttet til både strømningsteknikk varme- og massetransport og termodynamikk vurdere nøyaktigheten i beregningene og gyldigheten til den matematiske modellen</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>DAVE3710</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Akademisk Engelsk</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan på engelsk bruke korrekt terminologi innenfor teknologirelaterte emner generelt og innenfor et valgt fagområde spesielt presentere teknologi og relaterte prosesser utforme og skrive tekniske og akademiske tekster på engelsk i tråd med internasjonale konvensjoner og uttrykksmåte finne relevante kunnskapskilder vurdere kvaliteten på kilder og refererer til kilder i henhold til etablerte standarder bruke muntlig engelsk i faglige diskusjoner</t>
+        </is>
+      </c>
+      <c r="G5" s="1" t="inlineStr">
+        <is>
+          <t>EMTS2300</t>
+        </is>
+      </c>
+      <c r="H5" s="1" t="inlineStr">
+        <is>
+          <t>Varmetransport</t>
+        </is>
+      </c>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan bidra i arbeidet med å utvikle ny teknologi med bakgrunn i en forståelse for matematisk modellering og løsning av fysiske problemer løse koblede problemer knyttet til både varmetransport termodynamikk og fluidmekanikk strømningslære Dette vil være et grunnlag for beregning av for eksempel et byggs effekt- og energibehov vurdere om beregningsresultater er rimelige</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+      <c r="E6" s="1" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>EMVE3700</t>
+        </is>
+      </c>
+      <c r="H6" s="1" t="inlineStr">
+        <is>
+          <t>Numerisk varme- og strømningsteknikk</t>
+        </is>
+      </c>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>Studenten kan bidra i arbeidet med å utvikle ny teknologi med bakgrunn i en forståelse for matematisk modellering og løsning av fysiske problemer kan løse koblede problemer knyttet til både varmetransport termodynamikk og fluidmekanikk strømningslære Dette vil være et grunnlag for beregning av for eksempel et byggs effekt- og energibehov kan vurdere om beregningsresultater er rimelige sikre ferdigheter i en for fremtidens ingeniører aktuell arbeidsmåte</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
+      <c r="E7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>EMTS3900</t>
+        </is>
+      </c>
+      <c r="H7" s="1" t="inlineStr">
+        <is>
+          <t>Bacheloroppgave</t>
+        </is>
+      </c>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>Studenten behersker å arbeide i team med planlegging og gjennomføring av prosjekt viser selvstendighet og initiativ kreativitet og innovasjon vurderer teknologiske løsninger i en livsløps- miljømessig samfunnsmessig og økonomisk sammenheng analyserer og kvalitetssikrer resultatene og viser evne til refleksjon</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="50" customWidth="1" min="9" max="9"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LUK:</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>LUF:</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>LUG:</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Emnekode:</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Emnenavn:</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>Læringsutbytte</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>Emnekode:</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Emnenavn:</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>Læringsutbytte</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>Emnekode:</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>Emnenavn:</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Læringsutbytte</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
           <t>BEPE1700</t>
         </is>
       </c>

</xml_diff>

<commit_message>
skrevet i word-fil, endret småting i pptx
</commit_message>
<xml_diff>
--- a/resultat.xlsx
+++ b/resultat.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Statistikk" sheetId="1" state="visible" r:id="rId1"/>
@@ -239,10 +239,10 @@
                 <formatCode>General</formatCode>
                 <ptCount val="2"/>
                 <pt idx="0">
-                  <v>26</v>
+                  <v>59</v>
                 </pt>
                 <pt idx="1">
-                  <v>3286</v>
+                  <v>3721</v>
                 </pt>
               </numCache>
             </numRef>
@@ -365,10 +365,10 @@
                 <formatCode>General</formatCode>
                 <ptCount val="2"/>
                 <pt idx="0">
-                  <v>26</v>
+                  <v>59</v>
                 </pt>
                 <pt idx="1">
-                  <v>3286</v>
+                  <v>3721</v>
                 </pt>
               </numCache>
             </numRef>
@@ -867,7 +867,7 @@
   </sheetPr>
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
la inn unik emne funksjonalitet
</commit_message>
<xml_diff>
--- a/resultat.xlsx
+++ b/resultat.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Statistikk" sheetId="1" state="visible" r:id="rId1"/>
@@ -509,16 +509,16 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
-      <col>5</col>
-      <colOff>289560</colOff>
+      <col>6</col>
+      <colOff>19050</colOff>
       <row>5</row>
-      <rowOff>179070</rowOff>
+      <rowOff>91440</rowOff>
     </from>
     <to>
-      <col>9</col>
-      <colOff>960120</colOff>
+      <col>10</col>
+      <colOff>504825</colOff>
       <row>20</row>
-      <rowOff>179070</rowOff>
+      <rowOff>91440</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -537,15 +537,15 @@
   <twoCellAnchor>
     <from>
       <col>10</col>
-      <colOff>22860</colOff>
+      <colOff>533400</colOff>
       <row>5</row>
-      <rowOff>179070</rowOff>
+      <rowOff>91440</rowOff>
     </from>
     <to>
-      <col>14</col>
-      <colOff>601980</colOff>
+      <col>15</col>
+      <colOff>323850</colOff>
       <row>20</row>
-      <rowOff>179070</rowOff>
+      <rowOff>91440</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -867,14 +867,15 @@
   </sheetPr>
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col width="16.44140625" customWidth="1" min="1" max="1"/>
     <col width="13.5546875" customWidth="1" min="5" max="5"/>
+    <col width="12.5546875" customWidth="1" min="6" max="6"/>
     <col width="15.33203125" bestFit="1" customWidth="1" min="7" max="8"/>
     <col width="14.6640625" bestFit="1" customWidth="1" min="9" max="9"/>
     <col width="14.33203125" bestFit="1" customWidth="1" min="10" max="10"/>
@@ -909,6 +910,11 @@
           <t>Treff-søkeord</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Unike emner</t>
+        </is>
+      </c>
       <c r="G1" t="inlineStr">
         <is>
           <t>Totale treff</t>
@@ -961,6 +967,9 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
@@ -1004,6 +1013,9 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1023,6 +1035,9 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1042,6 +1057,9 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1061,6 +1079,9 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1080,6 +1101,9 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1099,6 +1123,9 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1118,6 +1145,9 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1137,6 +1167,9 @@
       <c r="E10" t="n">
         <v>5</v>
       </c>
+      <c r="F10" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1156,6 +1189,9 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1175,6 +1211,9 @@
       <c r="E12" t="n">
         <v>5</v>
       </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1194,6 +1233,9 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1213,6 +1255,9 @@
       <c r="E14" t="n">
         <v>5</v>
       </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1232,6 +1277,9 @@
       <c r="E15" t="n">
         <v>18</v>
       </c>
+      <c r="F15" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1251,6 +1299,9 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1270,6 +1321,9 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1289,6 +1343,9 @@
       <c r="E18" t="n">
         <v>0</v>
       </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1308,6 +1365,9 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1327,6 +1387,9 @@
       <c r="E20" t="n">
         <v>0</v>
       </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1346,6 +1409,9 @@
       <c r="E21" t="n">
         <v>0</v>
       </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1365,6 +1431,9 @@
       <c r="E22" t="n">
         <v>0</v>
       </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1384,6 +1453,9 @@
       <c r="E23" t="n">
         <v>0</v>
       </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1403,6 +1475,9 @@
       <c r="E24" t="n">
         <v>0</v>
       </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1422,6 +1497,9 @@
       <c r="E25" t="n">
         <v>0</v>
       </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1441,6 +1519,9 @@
       <c r="E26" t="n">
         <v>4</v>
       </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1460,6 +1541,9 @@
       <c r="E27" t="n">
         <v>10</v>
       </c>
+      <c r="F27" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1479,6 +1563,9 @@
       <c r="E28" t="n">
         <v>0</v>
       </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1498,6 +1585,9 @@
       <c r="E29" t="n">
         <v>0</v>
       </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1517,6 +1607,9 @@
       <c r="E30" t="n">
         <v>12</v>
       </c>
+      <c r="F30" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1534,6 +1627,9 @@
         <v>0</v>
       </c>
       <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>